<commit_message>
mise à jour mesures
</commit_message>
<xml_diff>
--- a/mesures.xlsx
+++ b/mesures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melvy\Desktop\Application\Drive\HEIG_VD\3em semestre\ASD2\Projet\ASD2_projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2B8AD1-94CC-49A4-AA9A-CC4F2E67EC05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710BBB47-6691-47EA-84B2-1C2F891F4422}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{323A6A3B-231C-4721-858D-A135CC06069E}"/>
   </bookViews>
@@ -333,7 +333,7 @@
                   <c:v>1243</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1753</c:v>
+                  <c:v>1610</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3311,8 +3311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0966656A-B49E-43E9-881F-416664C82BAD}">
   <dimension ref="B2:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3374,7 +3374,7 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7">
-        <v>1753</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -3498,6 +3498,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B3:D3"/>
@@ -3505,11 +3510,6 @@
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Ajustement main - Melvyn validation
</commit_message>
<xml_diff>
--- a/mesures.xlsx
+++ b/mesures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melvy\Desktop\Application\Drive\HEIG_VD\3em semestre\ASD2\Projet\ASD2_projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710BBB47-6691-47EA-84B2-1C2F891F4422}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DCA89E-7C76-4381-BA6F-522E5D2B7D26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{323A6A3B-231C-4721-858D-A135CC06069E}"/>
   </bookViews>
@@ -167,7 +167,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="fr-FR" baseline="0"/>
-              <a:t> du dictionnaire </a:t>
+              <a:t> du dictionnaire (moyenne de 4) </a:t>
             </a:r>
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
@@ -333,7 +333,7 @@
                   <c:v>1243</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1610</c:v>
+                  <c:v>1510</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3312,7 +3312,7 @@
   <dimension ref="B2:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3374,7 +3374,7 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7">
-        <v>1610</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -3498,11 +3498,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B3:D3"/>
@@ -3510,6 +3505,11 @@
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>